<commit_message>
1. Update Jplearn excel
</commit_message>
<xml_diff>
--- a/Daily.xlsx
+++ b/Daily.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="45" windowWidth="19395" windowHeight="7830"/>
@@ -11,12 +11,12 @@
     <sheet name="EN" sheetId="2" r:id="rId2"/>
     <sheet name="工作表3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="269">
   <si>
     <t>あいだがら</t>
   </si>
@@ -1048,6 +1048,334 @@
       </rPr>
       <t>　一朗剛打出全壘打</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>人柄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ひとがら</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>はながら</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>花柄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大柄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小柄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ごがら</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>取り柄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>とりえ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>人品</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>花紋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大個子、大花紋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小個子、小花紋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>おおがら</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>長處優點</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>柄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>え</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>器具把手、香菇根</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>横柄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>おうへい</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>傲慢、狂妄自大</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>相槌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>あいづち</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>隨聲附和(打つ)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>あいしょう</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>相性</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>合得來</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>相場</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>そうば</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>市價、匯率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>朝飯前</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>あさめしまえ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>早飯前、很容易</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>容易</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ようい</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>容易い</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>たやすい</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>簡單</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>簡單(形容)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>茶飯じ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>さはんじ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>常有的事</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本音</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ほんおん</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>真心話</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>先送り</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>さきおくり</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>延後</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>見合わせる</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>みあわせる</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>暫停延後</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>伸ばす</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>のばす</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>はやめる</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>早める</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提前</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>雨足</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>あまあし</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>雨勢</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大雨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小雨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>おおあめ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>こさめ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>春雨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>はるさめ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>風雨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ふうう</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>雨風</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>あめかぜ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>颳風下雨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>梅雨入り</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>梅雨明け</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>つゆいり</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>つゆあけ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>進入梅雨季</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出梅雨季</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>週明け</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>しゅうあけ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>年明け</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>としあけ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新年</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>周一(專業)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1385,7 +1713,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1440,6 +1768,57 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1452,64 +1831,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1815,8 +2146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1829,22 +2160,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18">
+      <c r="A1" s="35">
         <v>43802</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="18">
+      <c r="B1" s="36"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="35">
         <v>43806</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="20"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="37"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -2103,64 +2434,66 @@
       <c r="L11" s="11"/>
     </row>
     <row r="12" spans="1:12" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="37" t="s">
+      <c r="C12" s="32"/>
+      <c r="D12" s="20" t="s">
         <v>183</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="F12" s="38"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="36"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="32"/>
     </row>
     <row r="13" spans="1:12" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="32" t="s">
+      <c r="C13" s="34"/>
+      <c r="D13" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="F13" s="33"/>
+      <c r="F13" s="30"/>
       <c r="G13" s="12"/>
       <c r="H13" s="13"/>
       <c r="I13" s="14"/>
       <c r="J13" s="12"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="28"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="34"/>
     </row>
     <row r="14" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="18">
+      <c r="A14" s="35">
         <v>43803</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="20"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="35">
+        <v>43844</v>
+      </c>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="37"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
@@ -2172,9 +2505,15 @@
       <c r="C15" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
+      <c r="D15" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>196</v>
+      </c>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
@@ -2192,9 +2531,15 @@
       <c r="C16" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
+      <c r="D16" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>197</v>
+      </c>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
@@ -2212,9 +2557,15 @@
       <c r="C17" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
+      <c r="D17" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>198</v>
+      </c>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
@@ -2232,9 +2583,15 @@
       <c r="C18" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
+      <c r="D18" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>199</v>
+      </c>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
@@ -2252,9 +2609,15 @@
       <c r="C19" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
+      <c r="D19" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>201</v>
+      </c>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
@@ -2272,9 +2635,15 @@
       <c r="C20" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
+      <c r="D20" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>204</v>
+      </c>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
@@ -2292,9 +2661,15 @@
       <c r="C21" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
+      <c r="D21" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>207</v>
+      </c>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
@@ -2312,9 +2687,15 @@
       <c r="C22" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="D22" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>210</v>
+      </c>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
@@ -2330,9 +2711,15 @@
       <c r="C23" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
+      <c r="D23" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>213</v>
+      </c>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
@@ -2348,9 +2735,15 @@
       <c r="C24" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
+      <c r="D24" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>216</v>
+      </c>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
@@ -2362,53 +2755,57 @@
       <c r="A25" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="C25" s="22"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="22"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="24"/>
       <c r="G25" s="17"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="22"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="24"/>
       <c r="J25" s="17"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="22"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="24"/>
     </row>
     <row r="26" spans="1:12" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="C26" s="24"/>
+      <c r="C26" s="26"/>
       <c r="D26" s="11"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="24"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="26"/>
       <c r="G26" s="11"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="24"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="26"/>
       <c r="J26" s="11"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="24"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="26"/>
     </row>
     <row r="27" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="18">
+      <c r="A27" s="35">
         <v>43804</v>
       </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="20"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="35">
+        <v>43844</v>
+      </c>
+      <c r="E27" s="36"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="35">
+        <v>43844</v>
+      </c>
+      <c r="H27" s="36"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="35"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="37"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
@@ -2420,11 +2817,21 @@
       <c r="C28" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
+      <c r="D28" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>248</v>
+      </c>
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
@@ -2440,11 +2847,21 @@
       <c r="C29" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
+      <c r="D29" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>249</v>
+      </c>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
@@ -2460,11 +2877,21 @@
       <c r="C30" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
+      <c r="D30" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>251</v>
+      </c>
       <c r="I30" s="10"/>
       <c r="J30" s="10"/>
       <c r="K30" s="10"/>
@@ -2478,12 +2905,24 @@
       <c r="C31" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
+      <c r="D31" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>256</v>
+      </c>
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
       <c r="L31" s="10"/>
@@ -2498,12 +2937,24 @@
       <c r="C32" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
+      <c r="D32" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>256</v>
+      </c>
       <c r="J32" s="10"/>
       <c r="K32" s="10"/>
       <c r="L32" s="10"/>
@@ -2518,12 +2969,24 @@
       <c r="C33" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
+      <c r="D33" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="I33" s="10" t="s">
+        <v>261</v>
+      </c>
       <c r="J33" s="10"/>
       <c r="K33" s="10"/>
       <c r="L33" s="10"/>
@@ -2536,12 +2999,24 @@
       <c r="C34" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
+      <c r="D34" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>262</v>
+      </c>
       <c r="J34" s="10"/>
       <c r="K34" s="10"/>
       <c r="L34" s="10"/>
@@ -2556,12 +3031,24 @@
       <c r="C35" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
+      <c r="D35" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="I35" s="10" t="s">
+        <v>268</v>
+      </c>
       <c r="J35" s="10"/>
       <c r="K35" s="10"/>
       <c r="L35" s="10"/>
@@ -2576,12 +3063,24 @@
       <c r="C36" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
+      <c r="D36" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="I36" s="10" t="s">
+        <v>267</v>
+      </c>
       <c r="J36" s="10"/>
       <c r="K36" s="10"/>
       <c r="L36" s="10"/>
@@ -2596,9 +3095,15 @@
       <c r="C37" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
+      <c r="D37" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>245</v>
+      </c>
       <c r="G37" s="11"/>
       <c r="H37" s="11"/>
       <c r="I37" s="11"/>
@@ -2610,58 +3115,40 @@
       <c r="A38" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="38" t="s">
         <v>127</v>
       </c>
-      <c r="C38" s="22"/>
+      <c r="C38" s="24"/>
       <c r="D38" s="17"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="22"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="24"/>
       <c r="G38" s="17"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="22"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="24"/>
       <c r="J38" s="17"/>
-      <c r="K38" s="25"/>
-      <c r="L38" s="22"/>
+      <c r="K38" s="23"/>
+      <c r="L38" s="24"/>
     </row>
     <row r="39" spans="1:12" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="B39" s="27" t="s">
+      <c r="B39" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="C39" s="28"/>
+      <c r="C39" s="34"/>
       <c r="D39" s="11"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="24"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="26"/>
       <c r="G39" s="11"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="24"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="26"/>
       <c r="J39" s="11"/>
-      <c r="K39" s="26"/>
-      <c r="L39" s="24"/>
+      <c r="K39" s="25"/>
+      <c r="L39" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="K38:L38"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="H38:I38"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="A27:C27"/>
@@ -2678,6 +3165,24 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="G1:I1"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="H38:I38"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2700,16 +3205,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30">
+      <c r="A1" s="40">
         <v>43802</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="31"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="41"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -2852,16 +3357,16 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30">
+      <c r="A12" s="40">
         <v>43803</v>
       </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="31"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="41"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -3004,16 +3509,16 @@
       <c r="H22" s="4"/>
     </row>
     <row r="23" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="30">
+      <c r="A23" s="40">
         <v>43804</v>
       </c>
-      <c r="B23" s="31"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="31"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="41"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
@@ -3156,14 +3661,14 @@
       <c r="H33" s="4"/>
     </row>
     <row r="34" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="30"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="31"/>
+      <c r="A34" s="40"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="40"/>
+      <c r="H34" s="41"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
@@ -3266,14 +3771,14 @@
       <c r="H44" s="4"/>
     </row>
     <row r="45" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="30"/>
-      <c r="B45" s="31"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="30"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="30"/>
-      <c r="H45" s="31"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="41"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="41"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="41"/>
+      <c r="G45" s="40"/>
+      <c r="H45" s="41"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
@@ -3377,14 +3882,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:H34"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="G23:H23"/>
@@ -3397,6 +3894,14 @@
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="G12:H12"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:H34"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>